<commit_message>
feat: general statistics data
</commit_message>
<xml_diff>
--- a/downloads/download.xlsx
+++ b/downloads/download.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,18 +436,29 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Co-Authors Names</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Quantity of joint publications</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Affiliation</t>
-        </is>
+          <t>Indicators</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2017</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>2018</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>2022</v>
       </c>
     </row>
     <row r="2">
@@ -456,16 +467,29 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Semen A. Kurkin</t>
+          <t>Number of publications</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>18</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Immanuel Kant Baltic Federal University, Innopolis University</t>
-        </is>
+        <v>74</v>
+      </c>
+      <c r="D2" t="n">
+        <v>82</v>
+      </c>
+      <c r="E2" t="n">
+        <v>159</v>
+      </c>
+      <c r="F2" t="n">
+        <v>320</v>
+      </c>
+      <c r="G2" t="n">
+        <v>359</v>
+      </c>
+      <c r="H2" t="n">
+        <v>288</v>
+      </c>
+      <c r="I2" t="n">
+        <v>88</v>
       </c>
     </row>
     <row r="3">
@@ -474,16 +498,29 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Alexander K. Kuc</t>
+          <t>Articles</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Immanuel Kant Baltic Federal University, Yuri Gagarin State Technical University of Saratov, Innopolis University</t>
-        </is>
+        <v>16</v>
+      </c>
+      <c r="D3" t="n">
+        <v>22</v>
+      </c>
+      <c r="E3" t="n">
+        <v>48</v>
+      </c>
+      <c r="F3" t="n">
+        <v>89</v>
+      </c>
+      <c r="G3" t="n">
+        <v>87</v>
+      </c>
+      <c r="H3" t="n">
+        <v>114</v>
+      </c>
+      <c r="I3" t="n">
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -492,16 +529,29 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Andrey V. Andreev</t>
+          <t>Books</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Immanuel Kant Baltic Federal University, Innopolis University</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -510,16 +560,29 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Susanna Yu Gordleeva</t>
+          <t>Book Chapters</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Immanuel Kant Baltic Federal University, Lobachevsky State University of Nizhni Novgorod, Innopolis University</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +591,29 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Alexander E. Hramov</t>
+          <t>Conference Papers</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>44</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Lobachevsky State University of Nizhni Novgorod, Innolpolis University, Saint Petersburg State University, Saratov State Medical University named after V. I. Razumovsky, Innopolis University, Immanuel Kant Baltic Federal University</t>
-        </is>
+        <v>54</v>
+      </c>
+      <c r="D6" t="n">
+        <v>51</v>
+      </c>
+      <c r="E6" t="n">
+        <v>103</v>
+      </c>
+      <c r="F6" t="n">
+        <v>212</v>
+      </c>
+      <c r="G6" t="n">
+        <v>256</v>
+      </c>
+      <c r="H6" t="n">
+        <v>157</v>
+      </c>
+      <c r="I6" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -546,16 +622,29 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Nikita Frolov</t>
+          <t>Reviews</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Immanuel Kant Baltic Federal University, Innopolis University</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>7</v>
+      </c>
+      <c r="I7" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -564,16 +653,29 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Anastasiya E. Runnova</t>
+          <t>Short Surveys</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Saratov State Medical University named after V. I. Razumovsky, Yuri Gagarin State Technical University of Saratov, Innopolis University</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -582,16 +684,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Victor Borisovich Kazantsev</t>
+          <t>Others</t>
         </is>
       </c>
       <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" t="n">
+        <v>7</v>
+      </c>
+      <c r="I9" t="n">
         <v>2</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Immanuel Kant Baltic Federal University, Samara State Medical University, Lobachevsky State University of Nizhni Novgorod, Innopolis University</t>
-        </is>
       </c>
     </row>
     <row r="10">
@@ -600,16 +715,29 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Vladimir V. Makarov</t>
+          <t>Scopus</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Innopolis University</t>
-        </is>
+        <v>74</v>
+      </c>
+      <c r="D10" t="n">
+        <v>82</v>
+      </c>
+      <c r="E10" t="n">
+        <v>159</v>
+      </c>
+      <c r="F10" t="n">
+        <v>320</v>
+      </c>
+      <c r="G10" t="n">
+        <v>359</v>
+      </c>
+      <c r="H10" t="n">
+        <v>288</v>
+      </c>
+      <c r="I10" t="n">
+        <v>88</v>
       </c>
     </row>
     <row r="11">
@@ -618,16 +746,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Vadim V. Grubov</t>
+          <t>Q1 &amp; Q2</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>25</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Research and Production Company Immersmed, Saratov State Medical University named after V. I. Razumovsky, University of Innopolis, Innopolis University, Immanuel Kant Baltic Federal University</t>
-        </is>
+        <v>18</v>
+      </c>
+      <c r="D11" t="n">
+        <v>18</v>
+      </c>
+      <c r="E11" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" t="n">
+        <v>64</v>
+      </c>
+      <c r="G11" t="n">
+        <v>68</v>
+      </c>
+      <c r="H11" t="n">
+        <v>98</v>
+      </c>
+      <c r="I11" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -636,16 +777,29 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Nikita S. Frolov</t>
+          <t>Number of citations</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Immanuel Kant Baltic Federal University, Innopolis University</t>
-        </is>
+        <v>552</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1342</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1424</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2187</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1715</v>
+      </c>
+      <c r="H12" t="n">
+        <v>536</v>
+      </c>
+      <c r="I12" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="13">
@@ -654,16 +808,29 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Vladimir M. Antipov</t>
+          <t>&gt;10</t>
         </is>
       </c>
       <c r="C13" t="n">
+        <v>16</v>
+      </c>
+      <c r="D13" t="n">
+        <v>24</v>
+      </c>
+      <c r="E13" t="n">
+        <v>40</v>
+      </c>
+      <c r="F13" t="n">
+        <v>48</v>
+      </c>
+      <c r="G13" t="n">
+        <v>31</v>
+      </c>
+      <c r="H13" t="n">
+        <v>17</v>
+      </c>
+      <c r="I13" t="n">
         <v>1</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Innopolis University</t>
-        </is>
       </c>
     </row>
     <row r="14">
@@ -672,16 +839,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Natalya A. Aleksandrova</t>
+          <t>5-9</t>
         </is>
       </c>
       <c r="C14" t="n">
+        <v>23</v>
+      </c>
+      <c r="D14" t="n">
+        <v>21</v>
+      </c>
+      <c r="E14" t="n">
+        <v>49</v>
+      </c>
+      <c r="F14" t="n">
+        <v>60</v>
+      </c>
+      <c r="G14" t="n">
+        <v>75</v>
+      </c>
+      <c r="H14" t="n">
+        <v>32</v>
+      </c>
+      <c r="I14" t="n">
         <v>1</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Saratov State University</t>
-        </is>
       </c>
     </row>
     <row r="15">
@@ -690,16 +870,29 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Artem Badarin</t>
+          <t>1-4</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>9</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Immanuel Kant Baltic Federal University, Innopolis University</t>
-        </is>
+        <v>36</v>
+      </c>
+      <c r="D15" t="n">
+        <v>34</v>
+      </c>
+      <c r="E15" t="n">
+        <v>73</v>
+      </c>
+      <c r="F15" t="n">
+        <v>140</v>
+      </c>
+      <c r="G15" t="n">
+        <v>144</v>
+      </c>
+      <c r="H15" t="n">
+        <v>99</v>
+      </c>
+      <c r="I15" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="16">
@@ -708,160 +901,29 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Natalija A. Malova</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Innopolis University</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Alexey N. Pavlov</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>2</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Saratov State University, Yuri Gagarin State Technical University of Saratov</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Alexander N. Pisarchik</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>24</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Innolpolis University, Universidad Politécnica de Madrid, Innopolis University, Immanuel Kant Baltic Federal University, Centro de Tecnología Biomédica</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>V. S. Khorev</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>6</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Saratov State University, Innopolis University</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Muhammad Salman Kabir</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>1</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Innopolis University</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Elena N. Pitsik</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>11</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Immanuel Kant Baltic Federal University, Innopolis University</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Vladimir O. Nedaivozov</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>2</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Innopolis University</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Daniil V. Kirsanov</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Innopolis University</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Maksim O. Zhuravlev</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>4</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Saratov State University, Innopolis University</t>
-        </is>
+      <c r="D16" t="n">
+        <v>9</v>
+      </c>
+      <c r="E16" t="n">
+        <v>28</v>
+      </c>
+      <c r="F16" t="n">
+        <v>108</v>
+      </c>
+      <c r="G16" t="n">
+        <v>145</v>
+      </c>
+      <c r="H16" t="n">
+        <v>175</v>
+      </c>
+      <c r="I16" t="n">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>